<commit_message>
Operation Chaining 9ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining9nsSolution/power/OperationChaining9nsClockEnablePowerReport.xlsx
+++ b/reports/vivado/OperationChaining9nsSolution/power/OperationChaining9nsClockEnablePowerReport.xlsx
@@ -217,7 +217,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>3.70885303709656E-4</v>
+        <v>3.7110940320417285E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -243,16 +243,16 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>9.94720685412176E-5</v>
+        <v>9.978991147363558E-5</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>42.068965911865234</v>
+        <v>42.20338821411133</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>18.931034088134766</v>
+        <v>18.982187271118164</v>
       </c>
       <c r="E3" t="n" s="7">
         <v>105.0</v>
@@ -269,16 +269,16 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>9.859861893346533E-5</v>
+        <v>9.865831088973209E-5</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>38.620689392089844</v>
+        <v>38.64406967163086</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>17.379310607910156</v>
+        <v>17.38983154296875</v>
       </c>
       <c r="E4" t="n" s="7">
         <v>74.0</v>
@@ -295,16 +295,16 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>5.735000013373792E-5</v>
+        <v>5.7155593822244555E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>50.0</v>
+        <v>49.830509185791016</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>35.9151725769043</v>
+        <v>35.906951904296875</v>
       </c>
       <c r="E5" t="n" s="7">
         <v>34.0</v>
@@ -321,16 +321,16 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>2.6377241738373414E-5</v>
+        <v>2.646152461238671E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>42.068965911865234</v>
+        <v>42.20338821411133</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>18.931034088134766</v>
+        <v>18.964170455932617</v>
       </c>
       <c r="E6" t="n" s="7">
         <v>32.0</v>
@@ -347,16 +347,16 @@
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>2.5691035261843354E-5</v>
+        <v>2.5632543838582933E-5</v>
       </c>
       <c r="B7" t="s" s="4">
         <v>19</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>46.2068977355957</v>
+        <v>46.1016960144043</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>20.79310417175293</v>
+        <v>20.745763778686523</v>
       </c>
       <c r="E7" t="n" s="7">
         <v>10.0</v>
@@ -373,16 +373,16 @@
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>2.4748447685851716E-5</v>
+        <v>2.4724577087908983E-5</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>21</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>42.41379165649414</v>
+        <v>42.37288284301758</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>19.086206436157227</v>
+        <v>19.06779670715332</v>
       </c>
       <c r="E8" t="n" s="7">
         <v>32.0</v>
@@ -399,16 +399,16 @@
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>2.2895948859513737E-5</v>
+        <v>2.3012544261291623E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>23</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>38.44827651977539</v>
+        <v>38.64406967163086</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>17.27562141418457</v>
+        <v>17.38983154296875</v>
       </c>
       <c r="E9" t="n" s="7">
         <v>34.0</v>
@@ -425,16 +425,16 @@
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>5.136551862960914E-6</v>
+        <v>5.139661425346276E-6</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>24</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>38.620689392089844</v>
+        <v>38.64406967163086</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>17.379310607910156</v>
+        <v>17.38983154296875</v>
       </c>
       <c r="E10" t="n" s="7">
         <v>2.0</v>
@@ -451,16 +451,16 @@
     </row>
     <row r="11" outlineLevel="1">
       <c r="A11" t="n" s="5">
-        <v>4.944138254359132E-6</v>
+        <v>4.932881438435288E-6</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>25</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>46.2068977355957</v>
+        <v>46.1016960144043</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>17.379310607910156</v>
+        <v>17.38983154296875</v>
       </c>
       <c r="E11" t="n" s="7">
         <v>5.0</v>
@@ -477,16 +477,16 @@
     </row>
     <row r="12" outlineLevel="1">
       <c r="A12" t="n" s="5">
-        <v>4.3406894292274956E-6</v>
+        <v>4.26711858381168E-6</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>26</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>4.137930870056152</v>
+        <v>4.0677971839904785</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>1.862069010734558</v>
+        <v>1.8305089473724365</v>
       </c>
       <c r="E12" t="n" s="7">
         <v>35.0</v>
@@ -503,16 +503,16 @@
     </row>
     <row r="13" outlineLevel="1">
       <c r="A13" t="n" s="5">
-        <v>1.3306034816196188E-6</v>
+        <v>1.3347457752388436E-6</v>
       </c>
       <c r="B13" t="s" s="4">
         <v>27</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>42.24137878417969</v>
+        <v>42.37288284301758</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>18.758895874023438</v>
+        <v>18.86345672607422</v>
       </c>
       <c r="E13" t="n" s="7">
         <v>1.0</v>

</xml_diff>